<commit_message>
Print wifi debug message
debug for wifi timeout
</commit_message>
<xml_diff>
--- a/Watchy LUT.xlsx
+++ b/Watchy LUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/Watchy-CODE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C8027C0-7A6D-4DBA-BFAE-92C81F5771EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{8C8027C0-7A6D-4DBA-BFAE-92C81F5771EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{156E1CAF-9009-4D8E-8A3A-1EE75E9A4CEC}"/>
   <bookViews>
     <workbookView xWindow="12225" yWindow="3015" windowWidth="22875" windowHeight="16470" xr2:uid="{49CEF0DC-6239-4A6C-A42C-FB66DCC843CA}"/>
   </bookViews>
@@ -1057,16 +1057,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1394,7 +1394,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B21"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>